<commit_message>
TI Publication of RAD.IMR 1.0.0
</commit_message>
<xml_diff>
--- a/RAD/IMR/ValueSet-imr-servicerequest-intent-vs.xlsx
+++ b/RAD/IMR/ValueSet-imr-servicerequest-intent-vs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0-comment</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-03-18T08:53:35-05:00</t>
+    <t>2022-07-25T14:40:04-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>Copyright</t>
-  </si>
-  <si>
-    <t>IHE http://www.ihe.net/Governance/#Intellectual_Property</t>
   </si>
   <si>
     <t>Immutable</t>
@@ -402,16 +399,14 @@
       <c r="A16" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="B16" t="s" s="2">
-        <v>25</v>
-      </c>
+      <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s" s="2">
         <v>26</v>
-      </c>
-      <c r="B17" t="s" s="2">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -433,7 +428,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s" s="1">
         <v>21</v>
@@ -441,58 +436,58 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s" s="2">
         <v>29</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s" s="2">
         <v>31</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s" s="2">
         <v>33</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s" s="2">
         <v>35</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s" s="2">
         <v>37</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s" s="2">
         <v>40</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>